<commit_message>
Updated the simulated results with the smarter replacement algorithm
</commit_message>
<xml_diff>
--- a/simul-results.xlsx
+++ b/simul-results.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -378,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H122"/>
+  <dimension ref="A1:H159"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="I123" sqref="I123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.6"/>
@@ -3543,6 +3544,942 @@
       </c>
       <c r="H122">
         <v>1.8856085043517801</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8">
+      <c r="A124">
+        <v>0.5</v>
+      </c>
+      <c r="B124">
+        <v>0</v>
+      </c>
+      <c r="C124">
+        <v>4</v>
+      </c>
+      <c r="D124" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E124">
+        <v>4</v>
+      </c>
+      <c r="F124">
+        <v>0.29971483988425801</v>
+      </c>
+      <c r="G124">
+        <v>0.19492424740740599</v>
+      </c>
+      <c r="H124">
+        <v>0.17097107849536899</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8">
+      <c r="A125">
+        <v>0.5</v>
+      </c>
+      <c r="B125">
+        <v>4</v>
+      </c>
+      <c r="C125">
+        <v>4</v>
+      </c>
+      <c r="D125" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E125">
+        <v>4</v>
+      </c>
+      <c r="F125">
+        <v>0.57823282537037202</v>
+      </c>
+      <c r="G125">
+        <v>0.33600269710648001</v>
+      </c>
+      <c r="H125">
+        <v>0.251273154884257</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8">
+      <c r="A126">
+        <v>0.5</v>
+      </c>
+      <c r="B126">
+        <v>8</v>
+      </c>
+      <c r="C126">
+        <v>4</v>
+      </c>
+      <c r="D126" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E126">
+        <v>4</v>
+      </c>
+      <c r="F126">
+        <v>0.97179981273148996</v>
+      </c>
+      <c r="G126">
+        <v>0.52105919386573696</v>
+      </c>
+      <c r="H126">
+        <v>0.38930591321758901</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8">
+      <c r="A127">
+        <v>0.5</v>
+      </c>
+      <c r="B127">
+        <v>16</v>
+      </c>
+      <c r="C127">
+        <v>4</v>
+      </c>
+      <c r="D127" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E127">
+        <v>4</v>
+      </c>
+      <c r="F127">
+        <v>2.0033342421065399</v>
+      </c>
+      <c r="G127">
+        <v>1.02873470833335</v>
+      </c>
+      <c r="H127">
+        <v>0.66243425483796803</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8">
+      <c r="A128">
+        <v>0.5</v>
+      </c>
+      <c r="B128">
+        <v>0</v>
+      </c>
+      <c r="C128">
+        <v>16</v>
+      </c>
+      <c r="D128" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E128">
+        <v>4</v>
+      </c>
+      <c r="F128">
+        <v>7.8507939907407107E-2</v>
+      </c>
+      <c r="G128">
+        <v>6.55944978935184E-2</v>
+      </c>
+      <c r="H128">
+        <v>5.9843132962962897E-2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8">
+      <c r="A129">
+        <v>0.5</v>
+      </c>
+      <c r="B129">
+        <v>16</v>
+      </c>
+      <c r="C129">
+        <v>16</v>
+      </c>
+      <c r="D129" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E129">
+        <v>4</v>
+      </c>
+      <c r="F129">
+        <v>1.04169879129634</v>
+      </c>
+      <c r="G129">
+        <v>0.31487818692129299</v>
+      </c>
+      <c r="H129">
+        <v>0.25041225874999701</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8">
+      <c r="A130">
+        <v>0.5</v>
+      </c>
+      <c r="B130">
+        <v>32</v>
+      </c>
+      <c r="C130">
+        <v>16</v>
+      </c>
+      <c r="D130" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E130">
+        <v>4</v>
+      </c>
+      <c r="F130">
+        <v>1.4602245321297</v>
+      </c>
+      <c r="G130">
+        <v>0.66974825476854505</v>
+      </c>
+      <c r="H130">
+        <v>0.44397643495370998</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8">
+      <c r="A131">
+        <v>0.5</v>
+      </c>
+      <c r="B131">
+        <v>64</v>
+      </c>
+      <c r="C131">
+        <v>16</v>
+      </c>
+      <c r="D131" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E131">
+        <v>4</v>
+      </c>
+      <c r="F131">
+        <v>6.7798970750898304</v>
+      </c>
+      <c r="G131">
+        <v>1.3549492334258599</v>
+      </c>
+      <c r="H131">
+        <v>0.74276526891204098</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8">
+      <c r="A132">
+        <v>0.5</v>
+      </c>
+      <c r="B132">
+        <v>0</v>
+      </c>
+      <c r="C132">
+        <v>64</v>
+      </c>
+      <c r="D132" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E132">
+        <v>4</v>
+      </c>
+      <c r="F132">
+        <v>2.7599317245370299E-2</v>
+      </c>
+      <c r="G132">
+        <v>2.4191904814814799E-2</v>
+      </c>
+      <c r="H132">
+        <v>1.76881600694444E-2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8">
+      <c r="A133">
+        <v>0.5</v>
+      </c>
+      <c r="B133">
+        <v>64</v>
+      </c>
+      <c r="C133">
+        <v>64</v>
+      </c>
+      <c r="D133" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E133">
+        <v>4</v>
+      </c>
+      <c r="F133">
+        <v>1.03612105247665</v>
+      </c>
+      <c r="G133">
+        <v>0.302398810185182</v>
+      </c>
+      <c r="H133">
+        <v>0.225149659583331</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8">
+      <c r="A134">
+        <v>0.5</v>
+      </c>
+      <c r="B134">
+        <v>128</v>
+      </c>
+      <c r="C134">
+        <v>64</v>
+      </c>
+      <c r="D134" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E134">
+        <v>4</v>
+      </c>
+      <c r="F134">
+        <v>5.0064365696783302</v>
+      </c>
+      <c r="G134">
+        <v>2.5155529731466801</v>
+      </c>
+      <c r="H134">
+        <v>0.45670178201388301</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8">
+      <c r="A135">
+        <v>0.5</v>
+      </c>
+      <c r="B135">
+        <v>256</v>
+      </c>
+      <c r="C135">
+        <v>64</v>
+      </c>
+      <c r="D135" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E135">
+        <v>4</v>
+      </c>
+      <c r="F135">
+        <v>73.214955144815804</v>
+      </c>
+      <c r="G135">
+        <v>8.52171422177579</v>
+      </c>
+      <c r="H135">
+        <v>1.5470520565290899</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8">
+      <c r="A136">
+        <v>0.5</v>
+      </c>
+      <c r="B136">
+        <v>0</v>
+      </c>
+      <c r="C136">
+        <v>4</v>
+      </c>
+      <c r="D136" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E136">
+        <v>16</v>
+      </c>
+      <c r="F136">
+        <v>0.25082462076388801</v>
+      </c>
+      <c r="G136">
+        <v>0.202238247337962</v>
+      </c>
+      <c r="H136">
+        <v>0.168815220949073</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8">
+      <c r="A137">
+        <v>0.5</v>
+      </c>
+      <c r="B137">
+        <v>4</v>
+      </c>
+      <c r="C137">
+        <v>4</v>
+      </c>
+      <c r="D137" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E137">
+        <v>16</v>
+      </c>
+      <c r="F137">
+        <v>0.61168478944444404</v>
+      </c>
+      <c r="G137">
+        <v>0.33897604425925598</v>
+      </c>
+      <c r="H137">
+        <v>0.24599926175925699</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8">
+      <c r="A138">
+        <v>0.5</v>
+      </c>
+      <c r="B138">
+        <v>8</v>
+      </c>
+      <c r="C138">
+        <v>4</v>
+      </c>
+      <c r="D138" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E138">
+        <v>16</v>
+      </c>
+      <c r="F138">
+        <v>1.2781775546296399</v>
+      </c>
+      <c r="G138">
+        <v>0.53110780504629096</v>
+      </c>
+      <c r="H138">
+        <v>0.379980744166663</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8">
+      <c r="A139">
+        <v>0.5</v>
+      </c>
+      <c r="B139">
+        <v>16</v>
+      </c>
+      <c r="C139">
+        <v>4</v>
+      </c>
+      <c r="D139" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E139">
+        <v>16</v>
+      </c>
+      <c r="F139">
+        <v>4.3294177215051901</v>
+      </c>
+      <c r="G139">
+        <v>1.10253303997689</v>
+      </c>
+      <c r="H139">
+        <v>0.75965764263889801</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8">
+      <c r="A140">
+        <v>0.5</v>
+      </c>
+      <c r="B140">
+        <v>0</v>
+      </c>
+      <c r="C140">
+        <v>16</v>
+      </c>
+      <c r="D140" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E140">
+        <v>16</v>
+      </c>
+      <c r="F140">
+        <v>8.9236586689814601E-2</v>
+      </c>
+      <c r="G140">
+        <v>8.2711138680555393E-2</v>
+      </c>
+      <c r="H140">
+        <v>5.1089483194444403E-2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8">
+      <c r="A141">
+        <v>0.5</v>
+      </c>
+      <c r="B141">
+        <v>16</v>
+      </c>
+      <c r="C141">
+        <v>16</v>
+      </c>
+      <c r="D141" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E141">
+        <v>16</v>
+      </c>
+      <c r="F141">
+        <v>1.70628166925944</v>
+      </c>
+      <c r="G141">
+        <v>0.377332945972226</v>
+      </c>
+      <c r="H141">
+        <v>0.27754857303240998</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8">
+      <c r="A142">
+        <v>0.5</v>
+      </c>
+      <c r="B142">
+        <v>32</v>
+      </c>
+      <c r="C142">
+        <v>16</v>
+      </c>
+      <c r="D142" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E142">
+        <v>16</v>
+      </c>
+      <c r="F142">
+        <v>8.3326353867575396</v>
+      </c>
+      <c r="G142">
+        <v>0.48997288555555102</v>
+      </c>
+      <c r="H142">
+        <v>0.52439426208335904</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8">
+      <c r="A143">
+        <v>0.5</v>
+      </c>
+      <c r="B143">
+        <v>64</v>
+      </c>
+      <c r="C143">
+        <v>16</v>
+      </c>
+      <c r="D143" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E143">
+        <v>16</v>
+      </c>
+      <c r="F143">
+        <v>23.596685568222401</v>
+      </c>
+      <c r="G143">
+        <v>6.48037033015859</v>
+      </c>
+      <c r="H143">
+        <v>1.9062844804162999</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8">
+      <c r="A144">
+        <v>0.5</v>
+      </c>
+      <c r="B144">
+        <v>0</v>
+      </c>
+      <c r="C144">
+        <v>64</v>
+      </c>
+      <c r="D144" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E144">
+        <v>16</v>
+      </c>
+      <c r="F144">
+        <v>2.3757839537037001E-2</v>
+      </c>
+      <c r="G144">
+        <v>1.7731566597222199E-2</v>
+      </c>
+      <c r="H144">
+        <v>1.78111452314814E-2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8">
+      <c r="A145">
+        <v>0.5</v>
+      </c>
+      <c r="B145">
+        <v>64</v>
+      </c>
+      <c r="C145">
+        <v>64</v>
+      </c>
+      <c r="D145" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E145">
+        <v>16</v>
+      </c>
+      <c r="F145">
+        <v>6.5426804007908999</v>
+      </c>
+      <c r="G145">
+        <v>0.29914332060184901</v>
+      </c>
+      <c r="H145">
+        <v>0.225945445925924</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8">
+      <c r="A146">
+        <v>0.5</v>
+      </c>
+      <c r="B146">
+        <v>128</v>
+      </c>
+      <c r="C146">
+        <v>64</v>
+      </c>
+      <c r="D146" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E146">
+        <v>16</v>
+      </c>
+      <c r="F146">
+        <v>98.9561329835891</v>
+      </c>
+      <c r="G146">
+        <v>1.62032950984103</v>
+      </c>
+      <c r="H146">
+        <v>1.35553522155338</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8">
+      <c r="A147">
+        <v>0.5</v>
+      </c>
+      <c r="B147">
+        <v>256</v>
+      </c>
+      <c r="C147">
+        <v>64</v>
+      </c>
+      <c r="D147" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E147">
+        <v>16</v>
+      </c>
+      <c r="F147">
+        <v>261.92280178671399</v>
+      </c>
+      <c r="G147">
+        <v>213.649078346192</v>
+      </c>
+      <c r="H147">
+        <v>19.2613066836625</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8">
+      <c r="A148">
+        <v>0.5</v>
+      </c>
+      <c r="B148">
+        <v>0</v>
+      </c>
+      <c r="C148">
+        <v>4</v>
+      </c>
+      <c r="D148" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E148">
+        <v>64</v>
+      </c>
+      <c r="F148">
+        <v>0.27701322585648103</v>
+      </c>
+      <c r="G148">
+        <v>0.20126883488425701</v>
+      </c>
+      <c r="H148">
+        <v>0.174631695671295</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8">
+      <c r="A149">
+        <v>0.5</v>
+      </c>
+      <c r="B149">
+        <v>4</v>
+      </c>
+      <c r="C149">
+        <v>4</v>
+      </c>
+      <c r="D149" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E149">
+        <v>64</v>
+      </c>
+      <c r="F149">
+        <v>0.752271298495366</v>
+      </c>
+      <c r="G149">
+        <v>0.384654180324071</v>
+      </c>
+      <c r="H149">
+        <v>0.27900269171296099</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8">
+      <c r="A150">
+        <v>0.5</v>
+      </c>
+      <c r="B150">
+        <v>8</v>
+      </c>
+      <c r="C150">
+        <v>4</v>
+      </c>
+      <c r="D150" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E150">
+        <v>64</v>
+      </c>
+      <c r="F150">
+        <v>3.0110818942594499</v>
+      </c>
+      <c r="G150">
+        <v>2.1010495705555399</v>
+      </c>
+      <c r="H150">
+        <v>0.46214930124999398</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8">
+      <c r="A151">
+        <v>0.5</v>
+      </c>
+      <c r="B151">
+        <v>16</v>
+      </c>
+      <c r="C151">
+        <v>4</v>
+      </c>
+      <c r="D151" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E151">
+        <v>64</v>
+      </c>
+      <c r="F151">
+        <v>6.06406555666765</v>
+      </c>
+      <c r="G151">
+        <v>4.5111391500468896</v>
+      </c>
+      <c r="H151">
+        <v>3.82927323960689</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8">
+      <c r="A152">
+        <v>0.5</v>
+      </c>
+      <c r="B152">
+        <v>0</v>
+      </c>
+      <c r="C152">
+        <v>16</v>
+      </c>
+      <c r="D152" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E152">
+        <v>64</v>
+      </c>
+      <c r="F152">
+        <v>8.5084028865740499E-2</v>
+      </c>
+      <c r="G152">
+        <v>7.87539102314814E-2</v>
+      </c>
+      <c r="H152">
+        <v>4.7016504004629603E-2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8">
+      <c r="A153">
+        <v>0.5</v>
+      </c>
+      <c r="B153">
+        <v>16</v>
+      </c>
+      <c r="C153">
+        <v>16</v>
+      </c>
+      <c r="D153" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E153">
+        <v>64</v>
+      </c>
+      <c r="F153">
+        <v>9.3659350149287999</v>
+      </c>
+      <c r="G153">
+        <v>2.1138255585649302</v>
+      </c>
+      <c r="H153">
+        <v>0.844539107708416</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8">
+      <c r="A154">
+        <v>0.5</v>
+      </c>
+      <c r="B154">
+        <v>32</v>
+      </c>
+      <c r="C154">
+        <v>16</v>
+      </c>
+      <c r="D154" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E154">
+        <v>64</v>
+      </c>
+      <c r="F154">
+        <v>23.907027772990698</v>
+      </c>
+      <c r="G154">
+        <v>20.029920539778001</v>
+      </c>
+      <c r="H154">
+        <v>17.291851236401801</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8">
+      <c r="A155">
+        <v>0.5</v>
+      </c>
+      <c r="B155">
+        <v>64</v>
+      </c>
+      <c r="C155">
+        <v>16</v>
+      </c>
+      <c r="D155" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E155">
+        <v>64</v>
+      </c>
+      <c r="F155">
+        <v>69.997641602610102</v>
+      </c>
+      <c r="G155">
+        <v>57.206707278890299</v>
+      </c>
+      <c r="H155">
+        <v>54.261747995264898</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8">
+      <c r="A156">
+        <v>0.5</v>
+      </c>
+      <c r="B156">
+        <v>0</v>
+      </c>
+      <c r="C156">
+        <v>64</v>
+      </c>
+      <c r="D156" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E156">
+        <v>64</v>
+      </c>
+      <c r="F156">
+        <v>2.3085038356481399E-2</v>
+      </c>
+      <c r="G156">
+        <v>2.1884124421296201E-2</v>
+      </c>
+      <c r="H156">
+        <v>2.0719382592592501E-2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8">
+      <c r="A157">
+        <v>0.5</v>
+      </c>
+      <c r="B157">
+        <v>64</v>
+      </c>
+      <c r="C157">
+        <v>64</v>
+      </c>
+      <c r="D157" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E157">
+        <v>64</v>
+      </c>
+      <c r="F157">
+        <v>107.93493241173</v>
+      </c>
+      <c r="G157">
+        <v>8.8984467107919194</v>
+      </c>
+      <c r="H157">
+        <v>1.7038364348659301</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8">
+      <c r="A158">
+        <v>0.5</v>
+      </c>
+      <c r="B158">
+        <v>128</v>
+      </c>
+      <c r="C158">
+        <v>64</v>
+      </c>
+      <c r="D158" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E158">
+        <v>64</v>
+      </c>
+      <c r="F158">
+        <v>219.544538480131</v>
+      </c>
+      <c r="G158">
+        <v>231.16270800188599</v>
+      </c>
+      <c r="H158">
+        <v>227.643465886934</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8">
+      <c r="A159">
+        <v>0.5</v>
+      </c>
+      <c r="B159">
+        <v>256</v>
+      </c>
+      <c r="C159">
+        <v>64</v>
+      </c>
+      <c r="D159" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E159">
+        <v>64</v>
+      </c>
+      <c r="F159">
+        <v>477.00387594336701</v>
+      </c>
+      <c r="G159">
+        <v>459.159025543523</v>
+      </c>
+      <c r="H159">
+        <v>490.76132895169297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with the alternate method of wearout
</commit_message>
<xml_diff>
--- a/simul-results.xlsx
+++ b/simul-results.xlsx
@@ -79,9 +79,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -379,10 +382,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H159"/>
+  <dimension ref="A1:H168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="I123" sqref="I123"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="8" ySplit="2" topLeftCell="I161" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="I159" sqref="I159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.6"/>
@@ -406,23 +412,23 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -4480,6 +4486,214 @@
       </c>
       <c r="H159">
         <v>490.76132895169297</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8">
+      <c r="A161">
+        <v>0.5</v>
+      </c>
+      <c r="B161">
+        <v>0</v>
+      </c>
+      <c r="C161">
+        <v>4</v>
+      </c>
+      <c r="D161" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E161">
+        <v>4</v>
+      </c>
+      <c r="F161">
+        <v>17.912369254273202</v>
+      </c>
+      <c r="G161">
+        <v>9.7713736876360393</v>
+      </c>
+      <c r="H161">
+        <v>7.3548237699282701</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8">
+      <c r="A162">
+        <v>0.5</v>
+      </c>
+      <c r="B162">
+        <v>4</v>
+      </c>
+      <c r="C162">
+        <v>4</v>
+      </c>
+      <c r="D162" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E162">
+        <v>4</v>
+      </c>
+      <c r="F162">
+        <v>246.52939291626799</v>
+      </c>
+      <c r="G162">
+        <v>130.748737844918</v>
+      </c>
+      <c r="H162">
+        <v>87.520538552008304</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8">
+      <c r="A163">
+        <v>0.5</v>
+      </c>
+      <c r="B163">
+        <v>8</v>
+      </c>
+      <c r="C163">
+        <v>4</v>
+      </c>
+      <c r="D163" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E163">
+        <v>4</v>
+      </c>
+      <c r="F163">
+        <v>612.95055273015498</v>
+      </c>
+      <c r="G163">
+        <v>299.00767520110099</v>
+      </c>
+      <c r="H163">
+        <v>206.26904261756599</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8">
+      <c r="A164">
+        <v>0.5</v>
+      </c>
+      <c r="B164">
+        <v>16</v>
+      </c>
+      <c r="C164">
+        <v>4</v>
+      </c>
+      <c r="D164" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E164">
+        <v>4</v>
+      </c>
+      <c r="F164">
+        <v>1230.7247064841599</v>
+      </c>
+      <c r="G164">
+        <v>616.12638409976103</v>
+      </c>
+      <c r="H164">
+        <v>415.25637562513299</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8">
+      <c r="A165">
+        <v>0.5</v>
+      </c>
+      <c r="B165">
+        <v>0</v>
+      </c>
+      <c r="C165">
+        <v>16</v>
+      </c>
+      <c r="D165" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E165">
+        <v>4</v>
+      </c>
+      <c r="F165">
+        <v>6.1228669329616299</v>
+      </c>
+      <c r="G165">
+        <v>2.5146342016435401</v>
+      </c>
+      <c r="H165">
+        <v>1.68332685048621</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8">
+      <c r="A166">
+        <v>0.5</v>
+      </c>
+      <c r="B166">
+        <v>16</v>
+      </c>
+      <c r="C166">
+        <v>16</v>
+      </c>
+      <c r="D166" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E166">
+        <v>4</v>
+      </c>
+      <c r="F166">
+        <v>338.02622985043598</v>
+      </c>
+      <c r="G166">
+        <v>187.22995565284501</v>
+      </c>
+      <c r="H166">
+        <v>119.508993666872</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8">
+      <c r="A167">
+        <v>0.5</v>
+      </c>
+      <c r="B167">
+        <v>32</v>
+      </c>
+      <c r="C167">
+        <v>16</v>
+      </c>
+      <c r="D167" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E167">
+        <v>4</v>
+      </c>
+      <c r="F167">
+        <v>1677.2908399560799</v>
+      </c>
+      <c r="G167">
+        <v>847.08392392084204</v>
+      </c>
+      <c r="H167">
+        <v>542.53143373917305</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8">
+      <c r="A168">
+        <v>0.5</v>
+      </c>
+      <c r="B168">
+        <v>64</v>
+      </c>
+      <c r="C168">
+        <v>16</v>
+      </c>
+      <c r="D168" s="1">
+        <v>5.7875370370370305E-4</v>
+      </c>
+      <c r="E168">
+        <v>4</v>
+      </c>
+      <c r="F168">
+        <v>4331.0764879380404</v>
+      </c>
+      <c r="G168">
+        <v>2178.46998154115</v>
+      </c>
+      <c r="H168">
+        <v>1438.3704666875999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>